<commit_message>
multiple clinical scores / types
</commit_message>
<xml_diff>
--- a/public/MDS-UPDRSIII_Template.xlsx
+++ b/public/MDS-UPDRSIII_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/savirmadan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/savirmadan/Development/lead-dbs-programmer/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35FDA86-493B-7C44-898E-4895EA4B18EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06A1C2D-AC7D-E144-9A88-7529376C1437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="760" windowWidth="26300" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>PatientID</t>
   </si>
@@ -135,6 +135,9 @@
 # - Do not modify the column headings.
 # - Delete these instructions before uploading the file.
 </t>
+  </si>
+  <si>
+    <t>Score Type</t>
   </si>
 </sst>
 </file>
@@ -193,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -201,7 +204,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,42 +533,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AJ1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AJ7" sqref="AJ7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="41.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="40.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="28" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="30.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="30.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.2">
@@ -574,108 +576,110 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>